<commit_message>
Added SDV generative models
</commit_message>
<xml_diff>
--- a/cart_df.xlsx
+++ b/cart_df.xlsx
@@ -519,7 +519,7 @@
         <v>2.94</v>
       </c>
       <c r="E2">
-        <v>1500</v>
+        <v>1050</v>
       </c>
       <c r="F2">
         <v>30</v>
@@ -537,7 +537,7 @@
         <v>0</v>
       </c>
       <c r="K2">
-        <v>560</v>
+        <v>585</v>
       </c>
       <c r="L2">
         <v>585</v>
@@ -561,10 +561,10 @@
         <v>0.43</v>
       </c>
       <c r="S2">
-        <v>64.90000000000001</v>
+        <v>66.59999999999999</v>
       </c>
       <c r="T2">
-        <v>3.29</v>
+        <v>3.32</v>
       </c>
       <c r="U2">
         <v>0.4197407407407407</v>
@@ -602,7 +602,7 @@
         <v>0</v>
       </c>
       <c r="K3">
-        <v>560</v>
+        <v>585</v>
       </c>
       <c r="L3">
         <v>585</v>
@@ -626,10 +626,10 @@
         <v>0.25</v>
       </c>
       <c r="S3">
-        <v>59.7</v>
+        <v>62.3</v>
       </c>
       <c r="T3">
-        <v>5.28</v>
+        <v>6.01</v>
       </c>
       <c r="U3">
         <v>0.4197407407407407</v>
@@ -670,7 +670,7 @@
         <v>0</v>
       </c>
       <c r="L4">
-        <v>1115.2</v>
+        <v>780.6</v>
       </c>
       <c r="M4">
         <v>185</v>
@@ -682,16 +682,16 @@
         <v>5.82</v>
       </c>
       <c r="P4">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="Q4">
         <v>366</v>
       </c>
       <c r="R4">
-        <v>0.78</v>
+        <v>0.8</v>
       </c>
       <c r="S4">
-        <v>65</v>
+        <v>68.8</v>
       </c>
       <c r="T4">
         <v>4.61</v>
@@ -717,13 +717,13 @@
         <v>1120</v>
       </c>
       <c r="F5">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G5">
-        <v>0.45</v>
+        <v>0.43</v>
       </c>
       <c r="H5">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="I5">
         <v>730</v>
@@ -747,19 +747,19 @@
         <v>5.6</v>
       </c>
       <c r="P5">
-        <v>45.8</v>
+        <v>44.8</v>
       </c>
       <c r="Q5">
         <v>328</v>
       </c>
       <c r="R5">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="S5">
-        <v>189.3</v>
+        <v>159.2</v>
       </c>
       <c r="T5">
-        <v>6.37</v>
+        <v>7.41</v>
       </c>
       <c r="U5">
         <v>0.506</v>
@@ -800,7 +800,7 @@
         <v>585</v>
       </c>
       <c r="L6">
-        <v>560</v>
+        <v>585</v>
       </c>
       <c r="M6">
         <v>207</v>
@@ -821,10 +821,10 @@
         <v>0.25</v>
       </c>
       <c r="S6">
-        <v>61.5</v>
+        <v>62.3</v>
       </c>
       <c r="T6">
-        <v>4.87</v>
+        <v>5.94</v>
       </c>
       <c r="U6">
         <v>0.4197407407407407</v>
@@ -853,10 +853,10 @@
         <v>0.46</v>
       </c>
       <c r="H7">
-        <v>406</v>
+        <v>414</v>
       </c>
       <c r="I7">
-        <v>730</v>
+        <v>720</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -886,13 +886,13 @@
         <v>0.4</v>
       </c>
       <c r="S7">
-        <v>117.5</v>
+        <v>149.6</v>
       </c>
       <c r="T7">
-        <v>14.23</v>
+        <v>9.57</v>
       </c>
       <c r="U7">
-        <v>0.477</v>
+        <v>0.483</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -912,7 +912,7 @@
         <v>1050</v>
       </c>
       <c r="F8">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="G8">
         <v>0.47</v>
@@ -942,22 +942,22 @@
         <v>7</v>
       </c>
       <c r="P8">
-        <v>40.1</v>
+        <v>43</v>
       </c>
       <c r="Q8">
         <v>406.5</v>
       </c>
       <c r="R8">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="S8">
-        <v>70.8</v>
+        <v>73.40000000000001</v>
       </c>
       <c r="T8">
         <v>2.98</v>
       </c>
       <c r="U8">
-        <v>0.358</v>
+        <v>0.305</v>
       </c>
     </row>
     <row r="9" spans="1:21">
@@ -992,7 +992,7 @@
         <v>0</v>
       </c>
       <c r="K9">
-        <v>1120</v>
+        <v>1170</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -1010,16 +1010,16 @@
         <v>60.4</v>
       </c>
       <c r="Q9">
-        <v>321</v>
+        <v>343.1</v>
       </c>
       <c r="R9">
         <v>0.05</v>
       </c>
       <c r="S9">
-        <v>46.4</v>
+        <v>47</v>
       </c>
       <c r="T9">
-        <v>7.96</v>
+        <v>8.960000000000001</v>
       </c>
       <c r="U9">
         <v>0.4197407407407407</v>
@@ -1060,7 +1060,7 @@
         <v>0</v>
       </c>
       <c r="L10">
-        <v>780.6</v>
+        <v>1115.2</v>
       </c>
       <c r="M10">
         <v>204.8</v>
@@ -1072,7 +1072,7 @@
         <v>6.32</v>
       </c>
       <c r="P10">
-        <v>40.1</v>
+        <v>37.4</v>
       </c>
       <c r="Q10">
         <v>366.8</v>
@@ -1081,13 +1081,13 @@
         <v>0.8</v>
       </c>
       <c r="S10">
-        <v>49.7</v>
+        <v>46</v>
       </c>
       <c r="T10">
         <v>3.17</v>
       </c>
       <c r="U10">
-        <v>0.433</v>
+        <v>0.378</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -1122,7 +1122,7 @@
         <v>0</v>
       </c>
       <c r="K11">
-        <v>1115.2</v>
+        <v>1170</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -1143,13 +1143,13 @@
         <v>343.1</v>
       </c>
       <c r="R11">
-        <v>0.48</v>
+        <v>0.25</v>
       </c>
       <c r="S11">
-        <v>51.5</v>
+        <v>47</v>
       </c>
       <c r="T11">
-        <v>6.06</v>
+        <v>6.37</v>
       </c>
       <c r="U11">
         <v>0.4197407407407407</v>
@@ -1214,7 +1214,7 @@
         <v>54.5</v>
       </c>
       <c r="T12">
-        <v>8.68</v>
+        <v>8.67</v>
       </c>
       <c r="U12">
         <v>0.4197407407407407</v>
@@ -1246,7 +1246,7 @@
         <v>406</v>
       </c>
       <c r="I13">
-        <v>720</v>
+        <v>730</v>
       </c>
       <c r="J13">
         <v>0</v>
@@ -1270,19 +1270,19 @@
         <v>44.8</v>
       </c>
       <c r="Q13">
-        <v>321</v>
+        <v>382</v>
       </c>
       <c r="R13">
         <v>0.4</v>
       </c>
       <c r="S13">
-        <v>183.3</v>
+        <v>159.2</v>
       </c>
       <c r="T13">
         <v>4.85</v>
       </c>
       <c r="U13">
-        <v>0.5649999999999999</v>
+        <v>0.402</v>
       </c>
     </row>
     <row r="14" spans="1:21">
@@ -1332,22 +1332,22 @@
         <v>7</v>
       </c>
       <c r="P14">
-        <v>37.4</v>
+        <v>40.1</v>
       </c>
       <c r="Q14">
         <v>406.5</v>
       </c>
       <c r="R14">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="S14">
-        <v>69.59999999999999</v>
+        <v>73.90000000000001</v>
       </c>
       <c r="T14">
-        <v>3.04</v>
+        <v>3.32</v>
       </c>
       <c r="U14">
-        <v>0.338</v>
+        <v>0.402</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -1364,7 +1364,7 @@
         <v>2.94</v>
       </c>
       <c r="E15">
-        <v>1500</v>
+        <v>1050</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -1373,7 +1373,7 @@
         <v>0.5</v>
       </c>
       <c r="H15">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="I15">
         <v>630</v>
@@ -1403,13 +1403,13 @@
         <v>344.4</v>
       </c>
       <c r="R15">
-        <v>0.43</v>
+        <v>0.25</v>
       </c>
       <c r="S15">
-        <v>66.59999999999999</v>
+        <v>64.90000000000001</v>
       </c>
       <c r="T15">
-        <v>3.99</v>
+        <v>3.32</v>
       </c>
       <c r="U15">
         <v>0.4197407407407407</v>
@@ -1447,10 +1447,10 @@
         <v>0</v>
       </c>
       <c r="K16">
-        <v>336</v>
+        <v>334.6</v>
       </c>
       <c r="L16">
-        <v>1115.2</v>
+        <v>784</v>
       </c>
       <c r="M16">
         <v>204.8</v>
@@ -1462,7 +1462,7 @@
         <v>6.32</v>
       </c>
       <c r="P16">
-        <v>40.1</v>
+        <v>43</v>
       </c>
       <c r="Q16">
         <v>416</v>
@@ -1471,13 +1471,13 @@
         <v>0.8</v>
       </c>
       <c r="S16">
-        <v>63.6</v>
+        <v>54.5</v>
       </c>
       <c r="T16">
-        <v>3.18</v>
+        <v>3.58</v>
       </c>
       <c r="U16">
-        <v>0.356</v>
+        <v>0.378</v>
       </c>
     </row>
     <row r="17" spans="1:21">
@@ -1527,7 +1527,7 @@
         <v>6.32</v>
       </c>
       <c r="P17">
-        <v>40.6</v>
+        <v>40.1</v>
       </c>
       <c r="Q17">
         <v>416</v>
@@ -1536,13 +1536,13 @@
         <v>0.8</v>
       </c>
       <c r="S17">
-        <v>53.4</v>
+        <v>55</v>
       </c>
       <c r="T17">
-        <v>3.58</v>
+        <v>4.24</v>
       </c>
       <c r="U17">
-        <v>0.36</v>
+        <v>0.338</v>
       </c>
     </row>
     <row r="18" spans="1:21">
@@ -1562,7 +1562,7 @@
         <v>1500</v>
       </c>
       <c r="F18">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G18">
         <v>0.5</v>
@@ -1601,10 +1601,10 @@
         <v>0.43</v>
       </c>
       <c r="S18">
-        <v>66.59999999999999</v>
+        <v>63.8</v>
       </c>
       <c r="T18">
-        <v>3.99</v>
+        <v>3.29</v>
       </c>
       <c r="U18">
         <v>0.4197407407407407</v>
@@ -1630,7 +1630,7 @@
         <v>0</v>
       </c>
       <c r="G19">
-        <v>0.46</v>
+        <v>0.49</v>
       </c>
       <c r="H19">
         <v>400</v>
@@ -1642,7 +1642,7 @@
         <v>0</v>
       </c>
       <c r="K19">
-        <v>1170</v>
+        <v>1115.2</v>
       </c>
       <c r="L19">
         <v>0</v>
@@ -1663,7 +1663,7 @@
         <v>366</v>
       </c>
       <c r="R19">
-        <v>0.8</v>
+        <v>0.83</v>
       </c>
       <c r="S19">
         <v>65</v>
@@ -1692,7 +1692,7 @@
         <v>1120</v>
       </c>
       <c r="F20">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G20">
         <v>0.45</v>
@@ -1728,16 +1728,16 @@
         <v>328</v>
       </c>
       <c r="R20">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="S20">
-        <v>139.7</v>
+        <v>133.8</v>
       </c>
       <c r="T20">
-        <v>14.23</v>
+        <v>9.57</v>
       </c>
       <c r="U20">
-        <v>0.483</v>
+        <v>0.465</v>
       </c>
     </row>
     <row r="21" spans="1:21">
@@ -1757,7 +1757,7 @@
         <v>1500</v>
       </c>
       <c r="F21">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="G21">
         <v>0.5</v>
@@ -1796,7 +1796,7 @@
         <v>0.05</v>
       </c>
       <c r="S21">
-        <v>52.7</v>
+        <v>53.5</v>
       </c>
       <c r="T21">
         <v>7.96</v>
@@ -1858,16 +1858,16 @@
         <v>343.1</v>
       </c>
       <c r="R22">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="S22">
-        <v>39.8</v>
+        <v>49.7</v>
       </c>
       <c r="T22">
-        <v>8.68</v>
+        <v>8.67</v>
       </c>
       <c r="U22">
-        <v>0.46</v>
+        <v>0.4197407407407407</v>
       </c>
     </row>
     <row r="23" spans="1:21">
@@ -1923,16 +1923,16 @@
         <v>406.5</v>
       </c>
       <c r="R23">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="S23">
-        <v>70.8</v>
+        <v>71.40000000000001</v>
       </c>
       <c r="T23">
-        <v>2.98</v>
+        <v>3.07</v>
       </c>
       <c r="U23">
-        <v>0.36</v>
+        <v>0.402</v>
       </c>
     </row>
     <row r="24" spans="1:21">
@@ -1988,16 +1988,16 @@
         <v>366.8</v>
       </c>
       <c r="R24">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="S24">
         <v>42.1</v>
       </c>
       <c r="T24">
-        <v>3.32</v>
+        <v>3.08</v>
       </c>
       <c r="U24">
-        <v>0.402</v>
+        <v>0.338</v>
       </c>
     </row>
     <row r="25" spans="1:21">
@@ -2017,16 +2017,16 @@
         <v>1280</v>
       </c>
       <c r="F25">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G25">
-        <v>0.49</v>
+        <v>0.45</v>
       </c>
       <c r="H25">
         <v>406</v>
       </c>
       <c r="I25">
-        <v>720</v>
+        <v>730</v>
       </c>
       <c r="J25">
         <v>0</v>
@@ -2038,7 +2038,7 @@
         <v>585</v>
       </c>
       <c r="M25">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="N25">
         <v>55</v>
@@ -2047,19 +2047,19 @@
         <v>5.82</v>
       </c>
       <c r="P25">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Q25">
         <v>366</v>
       </c>
       <c r="R25">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="S25">
-        <v>65</v>
+        <v>67.59999999999999</v>
       </c>
       <c r="T25">
-        <v>4.87</v>
+        <v>8.890000000000001</v>
       </c>
       <c r="U25">
         <v>0.4197407407407407</v>
@@ -2121,10 +2121,10 @@
         <v>0.05</v>
       </c>
       <c r="S26">
-        <v>53.5</v>
+        <v>53.1</v>
       </c>
       <c r="T26">
-        <v>8.67</v>
+        <v>6.46</v>
       </c>
       <c r="U26">
         <v>0.4197407407407407</v>
@@ -2147,7 +2147,7 @@
         <v>1050</v>
       </c>
       <c r="F27">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="G27">
         <v>0.47</v>
@@ -2162,10 +2162,10 @@
         <v>0</v>
       </c>
       <c r="K27">
-        <v>609.9511111111112</v>
+        <v>780.6</v>
       </c>
       <c r="L27">
-        <v>334.6</v>
+        <v>292</v>
       </c>
       <c r="M27">
         <v>204.8</v>
@@ -2177,7 +2177,7 @@
         <v>6.32</v>
       </c>
       <c r="P27">
-        <v>40.1</v>
+        <v>43</v>
       </c>
       <c r="Q27">
         <v>416</v>
@@ -2189,10 +2189,10 @@
         <v>78.2</v>
       </c>
       <c r="T27">
-        <v>3.18</v>
+        <v>4.24</v>
       </c>
       <c r="U27">
-        <v>0.4197407407407407</v>
+        <v>0.406</v>
       </c>
     </row>
     <row r="28" spans="1:21">
@@ -2242,7 +2242,7 @@
         <v>7</v>
       </c>
       <c r="P28">
-        <v>40.6</v>
+        <v>37.4</v>
       </c>
       <c r="Q28">
         <v>406.5</v>
@@ -2251,13 +2251,13 @@
         <v>0.8</v>
       </c>
       <c r="S28">
-        <v>67</v>
+        <v>73.90000000000001</v>
       </c>
       <c r="T28">
-        <v>2.98</v>
+        <v>3.07</v>
       </c>
       <c r="U28">
-        <v>0.324</v>
+        <v>0.358</v>
       </c>
     </row>
     <row r="29" spans="1:21">
@@ -2316,13 +2316,13 @@
         <v>0.25</v>
       </c>
       <c r="S29">
-        <v>47</v>
+        <v>51.5</v>
       </c>
       <c r="T29">
-        <v>6.89</v>
+        <v>6.37</v>
       </c>
       <c r="U29">
-        <v>0.4197407407407407</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="30" spans="1:21">
@@ -2339,10 +2339,10 @@
         <v>2.94</v>
       </c>
       <c r="E30">
-        <v>1500</v>
+        <v>1050</v>
       </c>
       <c r="F30">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G30">
         <v>0.5</v>
@@ -2360,7 +2360,7 @@
         <v>585</v>
       </c>
       <c r="L30">
-        <v>585</v>
+        <v>560</v>
       </c>
       <c r="M30">
         <v>207</v>
@@ -2378,13 +2378,13 @@
         <v>344.4</v>
       </c>
       <c r="R30">
-        <v>0.43</v>
+        <v>0.48</v>
       </c>
       <c r="S30">
-        <v>63.6</v>
+        <v>63.8</v>
       </c>
       <c r="T30">
-        <v>3.71</v>
+        <v>3.29</v>
       </c>
       <c r="U30">
         <v>0.4197407407407407</v>
@@ -2446,10 +2446,10 @@
         <v>0.05</v>
       </c>
       <c r="S31">
-        <v>39.8</v>
+        <v>42.1</v>
       </c>
       <c r="T31">
-        <v>8.960000000000001</v>
+        <v>9.359999999999999</v>
       </c>
       <c r="U31">
         <v>0.4197407407407407</v>
@@ -2487,10 +2487,10 @@
         <v>0</v>
       </c>
       <c r="K32">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="L32">
-        <v>1115.2</v>
+        <v>780.6</v>
       </c>
       <c r="M32">
         <v>204.8</v>
@@ -2502,7 +2502,7 @@
         <v>6.32</v>
       </c>
       <c r="P32">
-        <v>40.1</v>
+        <v>43</v>
       </c>
       <c r="Q32">
         <v>416</v>
@@ -2511,13 +2511,13 @@
         <v>0.8</v>
       </c>
       <c r="S32">
-        <v>53.4</v>
+        <v>54.5</v>
       </c>
       <c r="T32">
-        <v>4.24</v>
+        <v>5.75</v>
       </c>
       <c r="U32">
-        <v>0.4197407407407407</v>
+        <v>0.356</v>
       </c>
     </row>
     <row r="33" spans="1:21">
@@ -2573,13 +2573,13 @@
         <v>344.4</v>
       </c>
       <c r="R33">
-        <v>0.25</v>
+        <v>0.05</v>
       </c>
       <c r="S33">
-        <v>62.3</v>
+        <v>59.6</v>
       </c>
       <c r="T33">
-        <v>6.01</v>
+        <v>5.94</v>
       </c>
       <c r="U33">
         <v>0.4197407407407407</v>
@@ -2602,25 +2602,25 @@
         <v>1280</v>
       </c>
       <c r="F34">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G34">
-        <v>0.46</v>
+        <v>0.45</v>
       </c>
       <c r="H34">
-        <v>400</v>
+        <v>406</v>
       </c>
       <c r="I34">
-        <v>700</v>
+        <v>730</v>
       </c>
       <c r="J34">
         <v>0</v>
       </c>
       <c r="K34">
-        <v>609.9511111111112</v>
+        <v>780.6</v>
       </c>
       <c r="L34">
-        <v>336</v>
+        <v>334.6</v>
       </c>
       <c r="M34">
         <v>185</v>
@@ -2632,19 +2632,19 @@
         <v>5.82</v>
       </c>
       <c r="P34">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="Q34">
         <v>366</v>
       </c>
       <c r="R34">
-        <v>0.85</v>
+        <v>0.8</v>
       </c>
       <c r="S34">
-        <v>67.59999999999999</v>
+        <v>65</v>
       </c>
       <c r="T34">
-        <v>5.44</v>
+        <v>4.88</v>
       </c>
       <c r="U34">
         <v>0.4197407407407407</v>
@@ -2682,7 +2682,7 @@
         <v>0</v>
       </c>
       <c r="K35">
-        <v>1170</v>
+        <v>1115.2</v>
       </c>
       <c r="L35">
         <v>0</v>
@@ -2709,7 +2709,7 @@
         <v>59.6</v>
       </c>
       <c r="T35">
-        <v>5.28</v>
+        <v>5.47</v>
       </c>
       <c r="U35">
         <v>0.4197407407407407</v>
@@ -2735,19 +2735,19 @@
         <v>100</v>
       </c>
       <c r="G36">
-        <v>0.45</v>
+        <v>0.43</v>
       </c>
       <c r="H36">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="I36">
-        <v>700</v>
+        <v>720</v>
       </c>
       <c r="J36">
         <v>0</v>
       </c>
       <c r="K36">
-        <v>334.6</v>
+        <v>0</v>
       </c>
       <c r="L36">
         <v>1115.2</v>
@@ -2762,22 +2762,22 @@
         <v>5.82</v>
       </c>
       <c r="P36">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q36">
         <v>366</v>
       </c>
       <c r="R36">
-        <v>0.8</v>
+        <v>0.72</v>
       </c>
       <c r="S36">
-        <v>65.2</v>
+        <v>67.59999999999999</v>
       </c>
       <c r="T36">
-        <v>4.88</v>
+        <v>4.78</v>
       </c>
       <c r="U36">
-        <v>0.417</v>
+        <v>0.4197407407407407</v>
       </c>
     </row>
     <row r="37" spans="1:21">
@@ -2839,7 +2839,7 @@
         <v>53.1</v>
       </c>
       <c r="T37">
-        <v>6.74</v>
+        <v>6.89</v>
       </c>
       <c r="U37">
         <v>0.4197407407407407</v>
@@ -2868,10 +2868,10 @@
         <v>0.49</v>
       </c>
       <c r="H38">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="I38">
-        <v>720</v>
+        <v>700</v>
       </c>
       <c r="J38">
         <v>0</v>
@@ -2898,7 +2898,7 @@
         <v>343.1</v>
       </c>
       <c r="R38">
-        <v>0.25</v>
+        <v>0.05</v>
       </c>
       <c r="S38">
         <v>139.7</v>
@@ -2907,7 +2907,7 @@
         <v>14.23</v>
       </c>
       <c r="U38">
-        <v>0.4197407407407407</v>
+        <v>0.406</v>
       </c>
     </row>
     <row r="39" spans="1:21">
@@ -2927,7 +2927,7 @@
         <v>1050</v>
       </c>
       <c r="F39">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="G39">
         <v>0.47</v>
@@ -2945,7 +2945,7 @@
         <v>0</v>
       </c>
       <c r="L39">
-        <v>1115.2</v>
+        <v>780.6</v>
       </c>
       <c r="M39">
         <v>204.8</v>
@@ -2957,22 +2957,22 @@
         <v>6.32</v>
       </c>
       <c r="P39">
-        <v>40.1</v>
+        <v>40.6</v>
       </c>
       <c r="Q39">
         <v>416</v>
       </c>
       <c r="R39">
-        <v>0.78</v>
+        <v>0.8</v>
       </c>
       <c r="S39">
         <v>52.9</v>
       </c>
       <c r="T39">
-        <v>4.24</v>
+        <v>3.58</v>
       </c>
       <c r="U39">
-        <v>0.356</v>
+        <v>0.4197407407407407</v>
       </c>
     </row>
     <row r="40" spans="1:21">
@@ -2992,7 +2992,7 @@
         <v>1050</v>
       </c>
       <c r="F40">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G40">
         <v>0.47</v>
@@ -3007,10 +3007,10 @@
         <v>0</v>
       </c>
       <c r="K40">
-        <v>780.6</v>
+        <v>609.9511111111112</v>
       </c>
       <c r="L40">
-        <v>334.6</v>
+        <v>336</v>
       </c>
       <c r="M40">
         <v>204.8</v>
@@ -3022,7 +3022,7 @@
         <v>7</v>
       </c>
       <c r="P40">
-        <v>37.4</v>
+        <v>40.1</v>
       </c>
       <c r="Q40">
         <v>406.5</v>
@@ -3031,13 +3031,13 @@
         <v>0.8</v>
       </c>
       <c r="S40">
-        <v>69.59999999999999</v>
+        <v>71.40000000000001</v>
       </c>
       <c r="T40">
-        <v>3.04</v>
+        <v>3.07</v>
       </c>
       <c r="U40">
-        <v>0.305</v>
+        <v>0.324</v>
       </c>
     </row>
     <row r="41" spans="1:21">
@@ -3060,13 +3060,13 @@
         <v>0</v>
       </c>
       <c r="G41">
-        <v>0.49</v>
+        <v>0.45</v>
       </c>
       <c r="H41">
         <v>406</v>
       </c>
       <c r="I41">
-        <v>730</v>
+        <v>720</v>
       </c>
       <c r="J41">
         <v>0</v>
@@ -3078,7 +3078,7 @@
         <v>0</v>
       </c>
       <c r="M41">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="N41">
         <v>55</v>
@@ -3096,10 +3096,10 @@
         <v>0.8</v>
       </c>
       <c r="S41">
-        <v>65.2</v>
+        <v>69.09999999999999</v>
       </c>
       <c r="T41">
-        <v>6.42</v>
+        <v>4.85</v>
       </c>
       <c r="U41">
         <v>0.4197407407407407</v>
@@ -3122,10 +3122,10 @@
         <v>1120</v>
       </c>
       <c r="F42">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G42">
-        <v>0.43</v>
+        <v>0.45</v>
       </c>
       <c r="H42">
         <v>414</v>
@@ -3137,7 +3137,7 @@
         <v>0</v>
       </c>
       <c r="K42">
-        <v>780.6</v>
+        <v>609.9511111111112</v>
       </c>
       <c r="L42">
         <v>535.0088888888888</v>
@@ -3152,13 +3152,13 @@
         <v>5.6</v>
       </c>
       <c r="P42">
-        <v>59.7</v>
+        <v>44.8</v>
       </c>
       <c r="Q42">
         <v>328</v>
       </c>
       <c r="R42">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="S42">
         <v>159.2</v>
@@ -3167,7 +3167,7 @@
         <v>6.06</v>
       </c>
       <c r="U42">
-        <v>0.572</v>
+        <v>0.501</v>
       </c>
     </row>
     <row r="43" spans="1:21">
@@ -3229,7 +3229,7 @@
         <v>39.1</v>
       </c>
       <c r="T43">
-        <v>7.49</v>
+        <v>9.41</v>
       </c>
       <c r="U43">
         <v>0.4197407407407407</v>
@@ -3285,19 +3285,19 @@
         <v>40.1</v>
       </c>
       <c r="Q44">
-        <v>366.8</v>
+        <v>416</v>
       </c>
       <c r="R44">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="S44">
-        <v>46</v>
+        <v>39.8</v>
       </c>
       <c r="T44">
-        <v>3.08</v>
+        <v>3.04</v>
       </c>
       <c r="U44">
-        <v>0.338</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="45" spans="1:21">
@@ -3332,10 +3332,10 @@
         <v>0</v>
       </c>
       <c r="K45">
+        <v>560</v>
+      </c>
+      <c r="L45">
         <v>585</v>
-      </c>
-      <c r="L45">
-        <v>560</v>
       </c>
       <c r="M45">
         <v>207</v>
@@ -3356,7 +3356,7 @@
         <v>0.05</v>
       </c>
       <c r="S45">
-        <v>59.7</v>
+        <v>61.4</v>
       </c>
       <c r="T45">
         <v>5.28</v>
@@ -3424,7 +3424,7 @@
         <v>52.7</v>
       </c>
       <c r="T46">
-        <v>8.68</v>
+        <v>7.96</v>
       </c>
       <c r="U46">
         <v>0.4197407407407407</v>
@@ -3447,7 +3447,7 @@
         <v>1050</v>
       </c>
       <c r="F47">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="G47">
         <v>0.47</v>
@@ -3477,7 +3477,7 @@
         <v>6.32</v>
       </c>
       <c r="P47">
-        <v>40.1</v>
+        <v>40.6</v>
       </c>
       <c r="Q47">
         <v>366.8</v>
@@ -3486,13 +3486,13 @@
         <v>0.8</v>
       </c>
       <c r="S47">
-        <v>42.1</v>
+        <v>46</v>
       </c>
       <c r="T47">
-        <v>3.17</v>
+        <v>3.19</v>
       </c>
       <c r="U47">
-        <v>0.4197407407407407</v>
+        <v>0.433</v>
       </c>
     </row>
     <row r="48" spans="1:21">
@@ -3551,10 +3551,10 @@
         <v>0.25</v>
       </c>
       <c r="S48">
-        <v>59.6</v>
+        <v>59.7</v>
       </c>
       <c r="T48">
-        <v>4.87</v>
+        <v>6.01</v>
       </c>
       <c r="U48">
         <v>0.4197407407407407</v>
@@ -3586,13 +3586,13 @@
         <v>406</v>
       </c>
       <c r="I49">
-        <v>730</v>
+        <v>700</v>
       </c>
       <c r="J49">
         <v>0</v>
       </c>
       <c r="K49">
-        <v>1170</v>
+        <v>1120</v>
       </c>
       <c r="L49">
         <v>0</v>
@@ -3607,7 +3607,7 @@
         <v>5.82</v>
       </c>
       <c r="P49">
-        <v>29.3</v>
+        <v>29</v>
       </c>
       <c r="Q49">
         <v>366</v>
@@ -3616,10 +3616,10 @@
         <v>0.85</v>
       </c>
       <c r="S49">
-        <v>68.8</v>
+        <v>67.59999999999999</v>
       </c>
       <c r="T49">
-        <v>8.890000000000001</v>
+        <v>7.03</v>
       </c>
       <c r="U49">
         <v>0.4197407407407407</v>
@@ -3743,13 +3743,13 @@
         <v>343.1</v>
       </c>
       <c r="R51">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="S51">
-        <v>39.8</v>
+        <v>50.4</v>
       </c>
       <c r="T51">
-        <v>9.359999999999999</v>
+        <v>7.49</v>
       </c>
       <c r="U51">
         <v>0.4197407407407407</v>
@@ -3808,7 +3808,7 @@
         <v>328</v>
       </c>
       <c r="R52">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="S52">
         <v>139.7</v>
@@ -3817,7 +3817,7 @@
         <v>9.130000000000001</v>
       </c>
       <c r="U52">
-        <v>0.477</v>
+        <v>0.465</v>
       </c>
     </row>
     <row r="53" spans="1:21">
@@ -3840,7 +3840,7 @@
         <v>50</v>
       </c>
       <c r="G53">
-        <v>0.43</v>
+        <v>0.45</v>
       </c>
       <c r="H53">
         <v>406</v>
@@ -3876,13 +3876,13 @@
         <v>0.4</v>
       </c>
       <c r="S53">
-        <v>189.3</v>
+        <v>183.3</v>
       </c>
       <c r="T53">
-        <v>14.23</v>
+        <v>9.84</v>
       </c>
       <c r="U53">
-        <v>0.533</v>
+        <v>0.477</v>
       </c>
     </row>
     <row r="54" spans="1:21">
@@ -3938,16 +3938,16 @@
         <v>321</v>
       </c>
       <c r="R54">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="S54">
-        <v>135.5</v>
+        <v>133.8</v>
       </c>
       <c r="T54">
-        <v>9.369999999999999</v>
+        <v>9.84</v>
       </c>
       <c r="U54">
-        <v>0.406</v>
+        <v>0.4197407407407407</v>
       </c>
     </row>
     <row r="55" spans="1:21">
@@ -4009,7 +4009,7 @@
         <v>54.9</v>
       </c>
       <c r="T55">
-        <v>8.68</v>
+        <v>7.49</v>
       </c>
       <c r="U55">
         <v>0.4197407407407407</v>
@@ -4035,10 +4035,10 @@
         <v>0</v>
       </c>
       <c r="G56">
-        <v>0.45</v>
+        <v>0.46</v>
       </c>
       <c r="H56">
-        <v>400</v>
+        <v>406</v>
       </c>
       <c r="I56">
         <v>710</v>
@@ -4068,13 +4068,13 @@
         <v>366</v>
       </c>
       <c r="R56">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="S56">
-        <v>65.2</v>
+        <v>65</v>
       </c>
       <c r="T56">
-        <v>6.42</v>
+        <v>4.87</v>
       </c>
       <c r="U56">
         <v>0.4197407407407407</v>
@@ -4127,22 +4127,22 @@
         <v>7</v>
       </c>
       <c r="P57">
-        <v>37.4</v>
+        <v>40.6</v>
       </c>
       <c r="Q57">
         <v>406.5</v>
       </c>
       <c r="R57">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="S57">
-        <v>70.8</v>
+        <v>73.40000000000001</v>
       </c>
       <c r="T57">
         <v>3.08</v>
       </c>
       <c r="U57">
-        <v>0.402</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="58" spans="1:21">
@@ -4180,7 +4180,7 @@
         <v>585</v>
       </c>
       <c r="L58">
-        <v>560</v>
+        <v>585</v>
       </c>
       <c r="M58">
         <v>207</v>
@@ -4201,10 +4201,10 @@
         <v>0.25</v>
       </c>
       <c r="S58">
-        <v>62.3</v>
+        <v>59.6</v>
       </c>
       <c r="T58">
-        <v>4.87</v>
+        <v>5.94</v>
       </c>
       <c r="U58">
         <v>0.4197407407407407</v>
@@ -4233,10 +4233,10 @@
         <v>0.45</v>
       </c>
       <c r="H59">
-        <v>406</v>
+        <v>414</v>
       </c>
       <c r="I59">
-        <v>730</v>
+        <v>720</v>
       </c>
       <c r="J59">
         <v>0</v>
@@ -4272,7 +4272,7 @@
         <v>9.84</v>
       </c>
       <c r="U59">
-        <v>0.465</v>
+        <v>0.533</v>
       </c>
     </row>
     <row r="60" spans="1:21">
@@ -4334,10 +4334,10 @@
         <v>69.59999999999999</v>
       </c>
       <c r="T60">
-        <v>2.8</v>
+        <v>2.98</v>
       </c>
       <c r="U60">
-        <v>0.335</v>
+        <v>0.338</v>
       </c>
     </row>
     <row r="61" spans="1:21">
@@ -4387,22 +4387,22 @@
         <v>7</v>
       </c>
       <c r="P61">
-        <v>40.1</v>
+        <v>37.4</v>
       </c>
       <c r="Q61">
         <v>406.5</v>
       </c>
       <c r="R61">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="S61">
-        <v>73.40000000000001</v>
+        <v>73.90000000000001</v>
       </c>
       <c r="T61">
-        <v>3.08</v>
+        <v>3.32</v>
       </c>
       <c r="U61">
-        <v>0.335</v>
+        <v>0.338</v>
       </c>
     </row>
     <row r="62" spans="1:21">
@@ -4422,7 +4422,7 @@
         <v>1050</v>
       </c>
       <c r="F62">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="G62">
         <v>0.47</v>
@@ -4452,7 +4452,7 @@
         <v>7</v>
       </c>
       <c r="P62">
-        <v>43</v>
+        <v>40.1</v>
       </c>
       <c r="Q62">
         <v>406.5</v>
@@ -4461,13 +4461,13 @@
         <v>0.5</v>
       </c>
       <c r="S62">
-        <v>73.40000000000001</v>
+        <v>70.8</v>
       </c>
       <c r="T62">
         <v>2.98</v>
       </c>
       <c r="U62">
-        <v>0.323</v>
+        <v>0.324</v>
       </c>
     </row>
     <row r="63" spans="1:21">
@@ -4523,16 +4523,16 @@
         <v>343.1</v>
       </c>
       <c r="R63">
-        <v>0.25</v>
+        <v>0.05</v>
       </c>
       <c r="S63">
         <v>46</v>
       </c>
       <c r="T63">
-        <v>4.61</v>
+        <v>4.55</v>
       </c>
       <c r="U63">
-        <v>0.4197407407407407</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="64" spans="1:21">
@@ -4567,7 +4567,7 @@
         <v>0</v>
       </c>
       <c r="K64">
-        <v>1170</v>
+        <v>1115.2</v>
       </c>
       <c r="L64">
         <v>0</v>
@@ -4588,13 +4588,13 @@
         <v>343.1</v>
       </c>
       <c r="R64">
-        <v>0.48</v>
+        <v>0.25</v>
       </c>
       <c r="S64">
-        <v>46.4</v>
+        <v>47</v>
       </c>
       <c r="T64">
-        <v>4.88</v>
+        <v>4.55</v>
       </c>
       <c r="U64">
         <v>0.4197407407407407</v>
@@ -4653,16 +4653,16 @@
         <v>406.5</v>
       </c>
       <c r="R65">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="S65">
-        <v>67</v>
+        <v>73.90000000000001</v>
       </c>
       <c r="T65">
-        <v>3.19</v>
+        <v>3.08</v>
       </c>
       <c r="U65">
-        <v>0.338</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="66" spans="1:21">
@@ -4712,22 +4712,22 @@
         <v>7</v>
       </c>
       <c r="P66">
-        <v>37.4</v>
+        <v>40.6</v>
       </c>
       <c r="Q66">
         <v>406.5</v>
       </c>
       <c r="R66">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="S66">
-        <v>67</v>
+        <v>69.59999999999999</v>
       </c>
       <c r="T66">
-        <v>3.19</v>
+        <v>3.17</v>
       </c>
       <c r="U66">
-        <v>0.338</v>
+        <v>0.335</v>
       </c>
     </row>
     <row r="67" spans="1:21">
@@ -4747,7 +4747,7 @@
         <v>1500</v>
       </c>
       <c r="F67">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="G67">
         <v>0.5</v>
@@ -4786,10 +4786,10 @@
         <v>0.05</v>
       </c>
       <c r="S67">
-        <v>52.7</v>
+        <v>53.5</v>
       </c>
       <c r="T67">
-        <v>7.49</v>
+        <v>8.960000000000001</v>
       </c>
       <c r="U67">
         <v>0.4197407407407407</v>
@@ -4812,7 +4812,7 @@
         <v>1050</v>
       </c>
       <c r="F68">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="G68">
         <v>0.47</v>
@@ -4848,16 +4848,16 @@
         <v>406.5</v>
       </c>
       <c r="R68">
-        <v>0.83</v>
+        <v>0.8</v>
       </c>
       <c r="S68">
         <v>67</v>
       </c>
       <c r="T68">
-        <v>3.07</v>
+        <v>2.98</v>
       </c>
       <c r="U68">
-        <v>0.358</v>
+        <v>0.323</v>
       </c>
     </row>
     <row r="69" spans="1:21">
@@ -4913,13 +4913,13 @@
         <v>344.4</v>
       </c>
       <c r="R69">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="S69">
-        <v>53.1</v>
+        <v>54.9</v>
       </c>
       <c r="T69">
-        <v>8.960000000000001</v>
+        <v>8.67</v>
       </c>
       <c r="U69">
         <v>0.4197407407407407</v>
@@ -4972,22 +4972,22 @@
         <v>6.32</v>
       </c>
       <c r="P70">
-        <v>40.1</v>
+        <v>43</v>
       </c>
       <c r="Q70">
-        <v>416</v>
+        <v>366.8</v>
       </c>
       <c r="R70">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="S70">
-        <v>49.7</v>
+        <v>50.4</v>
       </c>
       <c r="T70">
-        <v>3.19</v>
+        <v>3.04</v>
       </c>
       <c r="U70">
-        <v>0.36</v>
+        <v>0.338</v>
       </c>
     </row>
     <row r="71" spans="1:21">
@@ -5007,7 +5007,7 @@
         <v>1500</v>
       </c>
       <c r="F71">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="G71">
         <v>0.5</v>
@@ -5046,10 +5046,10 @@
         <v>0.05</v>
       </c>
       <c r="S71">
-        <v>52.7</v>
+        <v>53.1</v>
       </c>
       <c r="T71">
-        <v>9.359999999999999</v>
+        <v>7.96</v>
       </c>
       <c r="U71">
         <v>0.4197407407407407</v>
@@ -5072,7 +5072,7 @@
         <v>1050</v>
       </c>
       <c r="F72">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G72">
         <v>0.47</v>
@@ -5087,10 +5087,10 @@
         <v>0</v>
       </c>
       <c r="K72">
-        <v>780.6</v>
+        <v>609.9511111111112</v>
       </c>
       <c r="L72">
-        <v>334.6</v>
+        <v>292</v>
       </c>
       <c r="M72">
         <v>204.8</v>
@@ -5102,22 +5102,22 @@
         <v>7</v>
       </c>
       <c r="P72">
-        <v>40.6</v>
+        <v>40.1</v>
       </c>
       <c r="Q72">
         <v>406.5</v>
       </c>
       <c r="R72">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="S72">
-        <v>73.90000000000001</v>
+        <v>71.40000000000001</v>
       </c>
       <c r="T72">
         <v>3.07</v>
       </c>
       <c r="U72">
-        <v>0.305</v>
+        <v>0.358</v>
       </c>
     </row>
     <row r="73" spans="1:21">
@@ -5152,7 +5152,7 @@
         <v>0</v>
       </c>
       <c r="K73">
-        <v>609.9511111111112</v>
+        <v>784</v>
       </c>
       <c r="L73">
         <v>292</v>
@@ -5176,13 +5176,13 @@
         <v>0.8</v>
       </c>
       <c r="S73">
-        <v>71.40000000000001</v>
+        <v>73.40000000000001</v>
       </c>
       <c r="T73">
-        <v>2.98</v>
+        <v>3.04</v>
       </c>
       <c r="U73">
-        <v>0.323</v>
+        <v>0.324</v>
       </c>
     </row>
     <row r="74" spans="1:21">
@@ -5217,7 +5217,7 @@
         <v>0</v>
       </c>
       <c r="K74">
-        <v>560</v>
+        <v>585</v>
       </c>
       <c r="L74">
         <v>585</v>
@@ -5238,13 +5238,13 @@
         <v>344.4</v>
       </c>
       <c r="R74">
-        <v>0.43</v>
+        <v>0.48</v>
       </c>
       <c r="S74">
-        <v>63.6</v>
+        <v>64.90000000000001</v>
       </c>
       <c r="T74">
-        <v>3.32</v>
+        <v>3.71</v>
       </c>
       <c r="U74">
         <v>0.4197407407407407</v>
@@ -5270,13 +5270,13 @@
         <v>50</v>
       </c>
       <c r="G75">
-        <v>0.49</v>
+        <v>0.45</v>
       </c>
       <c r="H75">
-        <v>400</v>
+        <v>406</v>
       </c>
       <c r="I75">
-        <v>730</v>
+        <v>700</v>
       </c>
       <c r="J75">
         <v>0</v>
@@ -5300,19 +5300,19 @@
         <v>44.8</v>
       </c>
       <c r="Q75">
-        <v>343.1</v>
+        <v>321</v>
       </c>
       <c r="R75">
         <v>0.25</v>
       </c>
       <c r="S75">
-        <v>135.5</v>
+        <v>117.5</v>
       </c>
       <c r="T75">
-        <v>14.23</v>
+        <v>9.57</v>
       </c>
       <c r="U75">
-        <v>0.4197407407407407</v>
+        <v>0.406</v>
       </c>
     </row>
     <row r="76" spans="1:21">
@@ -5347,7 +5347,7 @@
         <v>0</v>
       </c>
       <c r="K76">
-        <v>1120</v>
+        <v>1170</v>
       </c>
       <c r="L76">
         <v>0</v>
@@ -5371,10 +5371,10 @@
         <v>0.43</v>
       </c>
       <c r="S76">
-        <v>61.5</v>
+        <v>61.4</v>
       </c>
       <c r="T76">
-        <v>6.01</v>
+        <v>4.87</v>
       </c>
       <c r="U76">
         <v>0.4197407407407407</v>
@@ -5412,7 +5412,7 @@
         <v>0</v>
       </c>
       <c r="K77">
-        <v>1120</v>
+        <v>1170</v>
       </c>
       <c r="L77">
         <v>0</v>
@@ -5433,13 +5433,13 @@
         <v>343.1</v>
       </c>
       <c r="R77">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="S77">
-        <v>53.1</v>
+        <v>54.5</v>
       </c>
       <c r="T77">
-        <v>6.74</v>
+        <v>6.37</v>
       </c>
       <c r="U77">
         <v>0.4197407407407407</v>
@@ -5495,16 +5495,16 @@
         <v>52.2</v>
       </c>
       <c r="Q78">
-        <v>343.1</v>
+        <v>321</v>
       </c>
       <c r="R78">
         <v>0.25</v>
       </c>
       <c r="S78">
-        <v>50.4</v>
+        <v>46</v>
       </c>
       <c r="T78">
-        <v>7.41</v>
+        <v>6.37</v>
       </c>
       <c r="U78">
         <v>0.4197407407407407</v>
@@ -5533,10 +5533,10 @@
         <v>0.46</v>
       </c>
       <c r="H79">
-        <v>400</v>
+        <v>406</v>
       </c>
       <c r="I79">
-        <v>700</v>
+        <v>720</v>
       </c>
       <c r="J79">
         <v>0</v>
@@ -5545,7 +5545,7 @@
         <v>585</v>
       </c>
       <c r="L79">
-        <v>560</v>
+        <v>585</v>
       </c>
       <c r="M79">
         <v>185</v>
@@ -5557,22 +5557,22 @@
         <v>5.82</v>
       </c>
       <c r="P79">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q79">
         <v>366</v>
       </c>
       <c r="R79">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="S79">
         <v>69.09999999999999</v>
       </c>
       <c r="T79">
-        <v>4.87</v>
+        <v>6.42</v>
       </c>
       <c r="U79">
-        <v>0.417</v>
+        <v>0.406</v>
       </c>
     </row>
     <row r="80" spans="1:21">
@@ -5592,7 +5592,7 @@
         <v>1500</v>
       </c>
       <c r="F80">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="G80">
         <v>0.5</v>
@@ -5631,10 +5631,10 @@
         <v>0.05</v>
       </c>
       <c r="S80">
-        <v>54.9</v>
+        <v>53.5</v>
       </c>
       <c r="T80">
-        <v>8.67</v>
+        <v>9.41</v>
       </c>
       <c r="U80">
         <v>0.4197407407407407</v>
@@ -5693,10 +5693,10 @@
         <v>343.1</v>
       </c>
       <c r="R81">
-        <v>0.43</v>
+        <v>0.48</v>
       </c>
       <c r="S81">
-        <v>47</v>
+        <v>53.1</v>
       </c>
       <c r="T81">
         <v>4.55</v>
@@ -5761,13 +5761,13 @@
         <v>0.8</v>
       </c>
       <c r="S82">
-        <v>63.6</v>
+        <v>55</v>
       </c>
       <c r="T82">
-        <v>5.75</v>
+        <v>3.18</v>
       </c>
       <c r="U82">
-        <v>0.402</v>
+        <v>0.338</v>
       </c>
     </row>
     <row r="83" spans="1:21">
@@ -5802,7 +5802,7 @@
         <v>0</v>
       </c>
       <c r="K83">
-        <v>1170</v>
+        <v>1115.2</v>
       </c>
       <c r="L83">
         <v>0</v>
@@ -5829,7 +5829,7 @@
         <v>46.4</v>
       </c>
       <c r="T83">
-        <v>4.88</v>
+        <v>4.61</v>
       </c>
       <c r="U83">
         <v>0.4197407407407407</v>
@@ -5891,10 +5891,10 @@
         <v>0.43</v>
       </c>
       <c r="S84">
-        <v>53.1</v>
+        <v>54.5</v>
       </c>
       <c r="T84">
-        <v>4.8</v>
+        <v>4.78</v>
       </c>
       <c r="U84">
         <v>0.4197407407407407</v>
@@ -5953,16 +5953,16 @@
         <v>328</v>
       </c>
       <c r="R85">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="S85">
-        <v>159.2</v>
+        <v>143.4</v>
       </c>
       <c r="T85">
-        <v>9.49</v>
+        <v>14.23</v>
       </c>
       <c r="U85">
-        <v>0.505</v>
+        <v>0.483</v>
       </c>
     </row>
     <row r="86" spans="1:21">
@@ -5988,7 +5988,7 @@
         <v>0.45</v>
       </c>
       <c r="H86">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="I86">
         <v>730</v>
@@ -6015,13 +6015,13 @@
         <v>44.8</v>
       </c>
       <c r="Q86">
-        <v>382</v>
+        <v>321</v>
       </c>
       <c r="R86">
         <v>0.4</v>
       </c>
       <c r="S86">
-        <v>117.5</v>
+        <v>149.6</v>
       </c>
       <c r="T86">
         <v>9.369999999999999</v>
@@ -6086,10 +6086,10 @@
         <v>0.05</v>
       </c>
       <c r="S87">
-        <v>54.9</v>
+        <v>53.1</v>
       </c>
       <c r="T87">
-        <v>7.49</v>
+        <v>9.359999999999999</v>
       </c>
       <c r="U87">
         <v>0.4197407407407407</v>
@@ -6148,7 +6148,7 @@
         <v>406.5</v>
       </c>
       <c r="R88">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="S88">
         <v>73.90000000000001</v>
@@ -6157,7 +6157,7 @@
         <v>2.98</v>
       </c>
       <c r="U88">
-        <v>0.402</v>
+        <v>0.335</v>
       </c>
     </row>
     <row r="89" spans="1:21">
@@ -6177,7 +6177,7 @@
         <v>1500</v>
       </c>
       <c r="F89">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="G89">
         <v>0.5</v>
@@ -6219,7 +6219,7 @@
         <v>53.1</v>
       </c>
       <c r="T89">
-        <v>7.41</v>
+        <v>6.89</v>
       </c>
       <c r="U89">
         <v>0.4197407407407407</v>
@@ -6281,7 +6281,7 @@
         <v>0.25</v>
       </c>
       <c r="S90">
-        <v>61.5</v>
+        <v>62.3</v>
       </c>
       <c r="T90">
         <v>4.87</v>
@@ -6304,7 +6304,7 @@
         <v>2.94</v>
       </c>
       <c r="E91">
-        <v>1050</v>
+        <v>1500</v>
       </c>
       <c r="F91">
         <v>0</v>
@@ -6313,7 +6313,7 @@
         <v>0.5</v>
       </c>
       <c r="H91">
-        <v>414</v>
+        <v>430</v>
       </c>
       <c r="I91">
         <v>630</v>
@@ -6322,7 +6322,7 @@
         <v>0</v>
       </c>
       <c r="K91">
-        <v>1115.2</v>
+        <v>1170</v>
       </c>
       <c r="L91">
         <v>0</v>
@@ -6346,10 +6346,10 @@
         <v>0.43</v>
       </c>
       <c r="S91">
-        <v>66.59999999999999</v>
+        <v>64.90000000000001</v>
       </c>
       <c r="T91">
-        <v>3.71</v>
+        <v>3.49</v>
       </c>
       <c r="U91">
         <v>0.4197407407407407</v>
@@ -6408,13 +6408,13 @@
         <v>343.1</v>
       </c>
       <c r="R92">
-        <v>0.25</v>
+        <v>0.48</v>
       </c>
       <c r="S92">
-        <v>46</v>
+        <v>42.1</v>
       </c>
       <c r="T92">
-        <v>6.06</v>
+        <v>7.41</v>
       </c>
       <c r="U92">
         <v>0.4197407407407407</v>
@@ -6452,7 +6452,7 @@
         <v>0</v>
       </c>
       <c r="K93">
-        <v>1115.2</v>
+        <v>1170</v>
       </c>
       <c r="L93">
         <v>0</v>
@@ -6473,13 +6473,13 @@
         <v>343.1</v>
       </c>
       <c r="R93">
-        <v>0.48</v>
+        <v>0.43</v>
       </c>
       <c r="S93">
-        <v>51.5</v>
+        <v>53.6</v>
       </c>
       <c r="T93">
-        <v>4.88</v>
+        <v>4.61</v>
       </c>
       <c r="U93">
         <v>0.4197407407407407</v>
@@ -6508,7 +6508,7 @@
         <v>0.5</v>
       </c>
       <c r="H94">
-        <v>414</v>
+        <v>430</v>
       </c>
       <c r="I94">
         <v>630</v>
@@ -6520,7 +6520,7 @@
         <v>878</v>
       </c>
       <c r="L94">
-        <v>334.6</v>
+        <v>292</v>
       </c>
       <c r="M94">
         <v>207</v>
@@ -6538,13 +6538,13 @@
         <v>344.4</v>
       </c>
       <c r="R94">
-        <v>0.48</v>
+        <v>0.43</v>
       </c>
       <c r="S94">
-        <v>63.6</v>
+        <v>64.90000000000001</v>
       </c>
       <c r="T94">
-        <v>3.29</v>
+        <v>3.32</v>
       </c>
       <c r="U94">
         <v>0.4197407407407407</v>
@@ -6567,16 +6567,16 @@
         <v>1280</v>
       </c>
       <c r="F95">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="G95">
-        <v>0.45</v>
+        <v>0.46</v>
       </c>
       <c r="H95">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="I95">
-        <v>720</v>
+        <v>710</v>
       </c>
       <c r="J95">
         <v>0</v>
@@ -6632,7 +6632,7 @@
         <v>1050</v>
       </c>
       <c r="F96">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="G96">
         <v>0.47</v>
@@ -6650,7 +6650,7 @@
         <v>0</v>
       </c>
       <c r="L96">
-        <v>1115.2</v>
+        <v>780.6</v>
       </c>
       <c r="M96">
         <v>204.8</v>
@@ -6671,13 +6671,13 @@
         <v>0.8</v>
       </c>
       <c r="S96">
-        <v>78.2</v>
+        <v>63.6</v>
       </c>
       <c r="T96">
-        <v>3.58</v>
+        <v>4.24</v>
       </c>
       <c r="U96">
-        <v>0.356</v>
+        <v>0.433</v>
       </c>
     </row>
     <row r="97" spans="1:21">
@@ -6697,7 +6697,7 @@
         <v>1500</v>
       </c>
       <c r="F97">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="G97">
         <v>0.5</v>
@@ -6736,10 +6736,10 @@
         <v>0.05</v>
       </c>
       <c r="S97">
-        <v>51.5</v>
+        <v>53.1</v>
       </c>
       <c r="T97">
-        <v>7.49</v>
+        <v>8.960000000000001</v>
       </c>
       <c r="U97">
         <v>0.4197407407407407</v>
@@ -6765,22 +6765,22 @@
         <v>100</v>
       </c>
       <c r="G98">
-        <v>0.43</v>
+        <v>0.45</v>
       </c>
       <c r="H98">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="I98">
-        <v>730</v>
+        <v>720</v>
       </c>
       <c r="J98">
         <v>0</v>
       </c>
       <c r="K98">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="L98">
-        <v>1115.2</v>
+        <v>780.6</v>
       </c>
       <c r="M98">
         <v>185</v>
@@ -6801,10 +6801,10 @@
         <v>0.8</v>
       </c>
       <c r="S98">
-        <v>65.2</v>
+        <v>68.8</v>
       </c>
       <c r="T98">
-        <v>4.78</v>
+        <v>4.55</v>
       </c>
       <c r="U98">
         <v>0.4197407407407407</v>
@@ -6842,7 +6842,7 @@
         <v>0</v>
       </c>
       <c r="K99">
-        <v>1170</v>
+        <v>1120</v>
       </c>
       <c r="L99">
         <v>0</v>
@@ -6863,13 +6863,13 @@
         <v>344.4</v>
       </c>
       <c r="R99">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="S99">
-        <v>53.1</v>
+        <v>53.5</v>
       </c>
       <c r="T99">
-        <v>8.960000000000001</v>
+        <v>9.41</v>
       </c>
       <c r="U99">
         <v>0.4197407407407407</v>
@@ -6922,22 +6922,22 @@
         <v>6.32</v>
       </c>
       <c r="P100">
-        <v>40.1</v>
+        <v>43</v>
       </c>
       <c r="Q100">
         <v>366.8</v>
       </c>
       <c r="R100">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="S100">
-        <v>49.7</v>
+        <v>39.8</v>
       </c>
       <c r="T100">
-        <v>3.08</v>
+        <v>3.32</v>
       </c>
       <c r="U100">
-        <v>0.36</v>
+        <v>0.338</v>
       </c>
     </row>
     <row r="101" spans="1:21">
@@ -6963,7 +6963,7 @@
         <v>0.45</v>
       </c>
       <c r="H101">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="I101">
         <v>730</v>
@@ -6990,19 +6990,19 @@
         <v>44.8</v>
       </c>
       <c r="Q101">
-        <v>321</v>
+        <v>382</v>
       </c>
       <c r="R101">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="S101">
         <v>117.5</v>
       </c>
       <c r="T101">
-        <v>9.49</v>
+        <v>14.23</v>
       </c>
       <c r="U101">
-        <v>0.477</v>
+        <v>0.533</v>
       </c>
     </row>
   </sheetData>

</xml_diff>